<commit_message>
small change in excel upload
</commit_message>
<xml_diff>
--- a/Server/uploads/fileGRADE.xlsx
+++ b/Server/uploads/fileGRADE.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mujahid\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unais\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2544BE82-35A8-4BCF-A0CF-548775A2F43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GRADE 8 BIO" sheetId="2" r:id="rId1"/>
@@ -361,7 +362,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -389,10 +390,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,26 +730,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D21"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="8" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="88" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -785,8 +784,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2">
@@ -795,30 +794,30 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3">
@@ -827,683 +826,683 @@
       <c r="C3">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1">
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" t="s">
         <v>31</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" t="s">
         <v>32</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1">
+    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1">
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>6</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="2" t="s">
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G7" t="s">
         <v>44</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="H7" t="s">
         <v>45</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" t="s">
         <v>46</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="J7" t="s">
         <v>47</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1">
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>7</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="2" t="s">
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" t="s">
         <v>50</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" t="s">
         <v>51</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" t="s">
         <v>52</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1">
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>8</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="2" t="s">
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" t="s">
         <v>56</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>9</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" t="s">
         <v>59</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" t="s">
         <v>60</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" t="s">
         <v>61</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" t="s">
         <v>62</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>10</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
         <v>67</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" t="s">
         <v>63</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="H11" t="s">
         <v>64</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" t="s">
         <v>65</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" t="s">
         <v>66</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1">
-        <v>11</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="2" t="s">
+    <row r="12" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
         <v>68</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" t="s">
         <v>69</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" t="s">
         <v>70</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" t="s">
         <v>71</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" t="s">
         <v>72</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1">
-        <v>12</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="2" t="s">
+    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" t="s">
         <v>85</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" t="s">
         <v>86</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" t="s">
         <v>87</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" t="s">
         <v>73</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1">
+    <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14">
         <v>13</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>13</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
         <v>74</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" t="s">
         <v>75</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" t="s">
         <v>76</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" t="s">
         <v>77</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" t="s">
         <v>14</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="1">
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
         <v>14</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>14</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
         <v>78</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G15" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" t="s">
         <v>79</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I15" t="s">
         <v>60</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J15" t="s">
         <v>61</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1">
+    <row r="16" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
         <v>15</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>15</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="2" t="s">
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
         <v>80</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="G16" t="s">
         <v>81</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" t="s">
         <v>82</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" t="s">
         <v>83</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" t="s">
         <v>84</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="1">
+    <row r="17" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17">
         <v>16</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>16</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="2" t="s">
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
         <v>89</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="G17" t="s">
         <v>90</v>
       </c>
-      <c r="H17" s="2" t="s">
+      <c r="H17" t="s">
         <v>91</v>
       </c>
-      <c r="I17" s="2" t="s">
+      <c r="I17" t="s">
         <v>92</v>
       </c>
-      <c r="J17" s="2" t="s">
+      <c r="J17" t="s">
         <v>93</v>
       </c>
-      <c r="K17" s="2" t="s">
+      <c r="K17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="1">
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18">
         <v>17</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>17</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
         <v>94</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" t="s">
         <v>95</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="H18" t="s">
         <v>96</v>
       </c>
-      <c r="I18" s="2" t="s">
+      <c r="I18" t="s">
         <v>77</v>
       </c>
-      <c r="J18" s="2" t="s">
+      <c r="J18" t="s">
         <v>14</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="K18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="1">
+    <row r="19" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19">
         <v>18</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>18</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
         <v>104</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" t="s">
         <v>105</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" t="s">
         <v>106</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" t="s">
         <v>107</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" t="s">
         <v>108</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="K19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="1">
+    <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20">
         <v>19</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
         <v>19</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="2" t="s">
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
         <v>97</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="G20" t="s">
         <v>98</v>
       </c>
-      <c r="H20" s="2" t="s">
+      <c r="H20" t="s">
         <v>49</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I20" t="s">
         <v>59</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="J20" t="s">
         <v>14</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="K20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="1">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21">
         <v>20</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21">
         <v>20</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
         <v>99</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" t="s">
         <v>100</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" t="s">
         <v>101</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I21" t="s">
         <v>102</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J21" t="s">
         <v>103</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>